<commit_message>
Changes to ALS and AWQC data import
</commit_message>
<xml_diff>
--- a/scripts/dataimport/ecology/UA_WQ_M/ConversionPH.xlsx
+++ b/scripts/dataimport/ecology/UA_WQ_M/ConversionPH.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00064235\Dropbox\MyWorkFolder\HCHB\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\scripts\dataimport\ecology\UA_WQ_M\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736524F0-1911-45A5-8EB2-C4C6C02032BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6225" windowWidth="16440" windowHeight="28590"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conversion" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="164">
   <si>
     <t>Old Name</t>
   </si>
@@ -508,12 +519,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_TOT_TDS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1355,11 +1369,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2687,7 +2701,7 @@
         <v>96</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>116</v>
@@ -2701,7 +2715,7 @@
         <v>97</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>116</v>
@@ -2838,5 +2852,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>